<commit_message>
Added ONE to the OceanCarrierRPAWithNames.xaml
</commit_message>
<xml_diff>
--- a/MultiProcess/Timestamps.xlsx
+++ b/MultiProcess/Timestamps.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pvanausdeln\OneDrive - Blume Global\UiPath\OceanCarrierRPA\MultiProcess\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sowrab.iyengar\Documents\OceanCarrierRPA\MultiProcess\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-51720" yWindow="-5670" windowWidth="51840" windowHeight="21240"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="6705"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="72">
+  <si>
+    <t>unitid</t>
+  </si>
+  <si>
+    <t>timestamps</t>
+  </si>
   <si>
     <t>NYKU5921650</t>
   </si>
@@ -186,16 +192,58 @@
     <t>UNIT1207192</t>
   </si>
   <si>
-    <t>unitid</t>
-  </si>
-  <si>
-    <t>timestamps</t>
+    <t>OOLU6456762</t>
+  </si>
+  <si>
+    <t>CAIU5557752</t>
+  </si>
+  <si>
+    <t>FSCU4842990</t>
+  </si>
+  <si>
+    <t>APRU5077315</t>
+  </si>
+  <si>
+    <t>APZU3750590</t>
+  </si>
+  <si>
+    <t>TCNU4714233</t>
+  </si>
+  <si>
+    <t>TCLU6542033</t>
+  </si>
+  <si>
+    <t>APHU7406718</t>
+  </si>
+  <si>
+    <t>TGHU1104199</t>
+  </si>
+  <si>
+    <t>TCKU9947531</t>
+  </si>
+  <si>
+    <t>TEST87987977</t>
+  </si>
+  <si>
+    <t>GESU6346823</t>
+  </si>
+  <si>
+    <t>UETU4070902</t>
+  </si>
+  <si>
+    <t>UNIT0801001</t>
+  </si>
+  <si>
+    <t>OOLU6268132</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -245,11 +293,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -553,52 +602,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B338"/>
+  <dimension ref="A1:B353"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B1" t="s">
-        <v>56</v>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1">
+        <v>2</v>
+      </c>
+      <c r="B2">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>43677.707048611112</v>
+        <v>43680.576898148145</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B4" s="2">
-        <v>43677.707152777781</v>
+        <v>43680.576793981483</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -606,7 +650,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -614,7 +658,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -622,7 +666,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -630,7 +674,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -638,7 +682,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -646,7 +690,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -654,7 +698,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -662,7 +706,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -670,7 +714,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -678,7 +722,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -686,7 +730,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -694,7 +738,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -702,7 +746,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -710,7 +754,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -718,7 +762,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -726,7 +770,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -734,7 +778,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -742,7 +786,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -750,7 +794,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -758,7 +802,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -766,7 +810,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -774,7 +818,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -782,7 +826,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -790,7 +834,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -798,7 +842,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -806,7 +850,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -814,7 +858,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -822,7 +866,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -830,7 +874,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -838,7 +882,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -846,7 +890,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -854,7 +898,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -862,7 +906,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -870,7 +914,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -878,7 +922,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -886,7 +930,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -894,7 +938,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -902,7 +946,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -910,7 +954,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -918,7 +962,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -926,7 +970,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -934,7 +978,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -942,15 +986,15 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B48">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="B48" s="2">
+        <v>43679.633379629631</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -958,7 +1002,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -966,7 +1010,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -974,7 +1018,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -982,7 +1026,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -990,23 +1034,23 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B54">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="B54" s="2">
+        <v>43679.633831018517</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B55">
-        <v>0</v>
+        <v>13</v>
+      </c>
+      <c r="B55" s="2">
+        <v>43679.633530092593</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B56">
         <v>0</v>
@@ -1014,7 +1058,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B57">
         <v>0</v>
@@ -1022,7 +1066,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B58">
         <v>0</v>
@@ -1030,15 +1074,15 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B59">
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="B59" s="2">
+        <v>43679.633935185186</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B60">
         <v>0</v>
@@ -1046,7 +1090,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B61">
         <v>0</v>
@@ -1054,15 +1098,15 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B62">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="B62" s="2">
+        <v>43679.634097222224</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B63">
         <v>0</v>
@@ -1070,7 +1114,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B64">
         <v>0</v>
@@ -1078,7 +1122,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B65">
         <v>0</v>
@@ -1086,7 +1130,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B66">
         <v>0</v>
@@ -1094,7 +1138,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B67">
         <v>0</v>
@@ -1102,7 +1146,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B68">
         <v>0</v>
@@ -1110,7 +1154,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B69">
         <v>0</v>
@@ -1118,7 +1162,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B70">
         <v>0</v>
@@ -1126,7 +1170,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B71">
         <v>0</v>
@@ -1134,7 +1178,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B72">
         <v>0</v>
@@ -1142,7 +1186,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B73">
         <v>0</v>
@@ -1150,7 +1194,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B74">
         <v>0</v>
@@ -1158,7 +1202,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B75">
         <v>0</v>
@@ -1166,7 +1210,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B76">
         <v>0</v>
@@ -1174,7 +1218,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B77">
         <v>0</v>
@@ -1182,39 +1226,39 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B78">
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="B78" s="2">
+        <v>43679.636064814818</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B79">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="B79" s="2">
+        <v>43679.63585648148</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B80">
-        <v>0</v>
+        <v>18</v>
+      </c>
+      <c r="B80" s="2">
+        <v>43679.635752314818</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B81">
-        <v>0</v>
+        <v>19</v>
+      </c>
+      <c r="B81" s="2">
+        <v>43679.63553240741</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B82">
         <v>0</v>
@@ -1222,7 +1266,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B83">
         <v>0</v>
@@ -1230,15 +1274,15 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B84">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="B84" s="2">
+        <v>43679.636469907404</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B85">
         <v>0</v>
@@ -1246,39 +1290,39 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B86">
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="B86" s="2">
+        <v>43679.637002314812</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B87">
-        <v>0</v>
+        <v>22</v>
+      </c>
+      <c r="B87" s="2">
+        <v>43679.637291666666</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B88">
-        <v>0</v>
+        <v>23</v>
+      </c>
+      <c r="B88" s="2">
+        <v>43679.637164351851</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B89">
-        <v>0</v>
+        <v>24</v>
+      </c>
+      <c r="B89" s="2">
+        <v>43679.637673611112</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B90">
         <v>0</v>
@@ -1286,7 +1330,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B91">
         <v>0</v>
@@ -1294,7 +1338,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B92">
         <v>0</v>
@@ -1302,7 +1346,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B93">
         <v>0</v>
@@ -1310,7 +1354,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B94">
         <v>0</v>
@@ -1318,7 +1362,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B95">
         <v>0</v>
@@ -1326,23 +1370,23 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B96">
-        <v>0</v>
+        <v>25</v>
+      </c>
+      <c r="B96" s="2">
+        <v>43679.635277777779</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B97">
-        <v>0</v>
+        <v>26</v>
+      </c>
+      <c r="B97" s="2">
+        <v>43679.634629629632</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B98">
         <v>0</v>
@@ -1350,7 +1394,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B99">
         <v>0</v>
@@ -1358,7 +1402,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B100">
         <v>0</v>
@@ -1366,7 +1410,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B101">
         <v>0</v>
@@ -1374,7 +1418,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B102">
         <v>0</v>
@@ -1382,7 +1426,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B103">
         <v>0</v>
@@ -1390,7 +1434,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B104">
         <v>0</v>
@@ -1398,7 +1442,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B105">
         <v>0</v>
@@ -1406,7 +1450,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B106">
         <v>0</v>
@@ -1414,31 +1458,31 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B107">
-        <v>0</v>
+        <v>27</v>
+      </c>
+      <c r="B107" s="2">
+        <v>43679.634340277778</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B108">
-        <v>0</v>
+        <v>28</v>
+      </c>
+      <c r="B108" s="2">
+        <v>43679.634444444448</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B109">
-        <v>0</v>
+        <v>29</v>
+      </c>
+      <c r="B109" s="2">
+        <v>43679.634942129633</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B110">
         <v>0</v>
@@ -1446,7 +1490,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B111">
         <v>0</v>
@@ -1454,15 +1498,15 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B112">
-        <v>0</v>
+        <v>30</v>
+      </c>
+      <c r="B112" s="2">
+        <v>43679.635405092595</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B113">
         <v>0</v>
@@ -1470,7 +1514,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B114">
         <v>0</v>
@@ -1478,7 +1522,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B115">
         <v>0</v>
@@ -1486,7 +1530,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B116">
         <v>0</v>
@@ -1494,7 +1538,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B117">
         <v>0</v>
@@ -1502,7 +1546,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B118">
         <v>0</v>
@@ -1510,7 +1554,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B119">
         <v>0</v>
@@ -1518,7 +1562,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B120">
         <v>0</v>
@@ -1526,7 +1570,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B121">
         <v>0</v>
@@ -1534,7 +1578,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B122">
         <v>0</v>
@@ -1542,7 +1586,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B123">
         <v>0</v>
@@ -1550,7 +1594,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B124">
         <v>0</v>
@@ -1558,7 +1602,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B125">
         <v>0</v>
@@ -1566,7 +1610,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B126">
         <v>0</v>
@@ -1574,7 +1618,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B127">
         <v>0</v>
@@ -1582,7 +1626,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B128">
         <v>0</v>
@@ -1590,7 +1634,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B129">
         <v>0</v>
@@ -1598,7 +1642,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B130">
         <v>0</v>
@@ -1606,7 +1650,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B131">
         <v>0</v>
@@ -1614,7 +1658,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B132">
         <v>0</v>
@@ -1622,7 +1666,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B133">
         <v>0</v>
@@ -1630,7 +1674,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B134">
         <v>0</v>
@@ -1638,7 +1682,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B135">
         <v>0</v>
@@ -1646,7 +1690,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B136">
         <v>0</v>
@@ -1654,7 +1698,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B137">
         <v>0</v>
@@ -1662,7 +1706,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B138">
         <v>0</v>
@@ -1670,7 +1714,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B139">
         <v>0</v>
@@ -1678,7 +1722,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B140">
         <v>0</v>
@@ -1686,7 +1730,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B141">
         <v>0</v>
@@ -1694,7 +1738,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B142">
         <v>0</v>
@@ -1702,7 +1746,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B143">
         <v>0</v>
@@ -1710,7 +1754,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B144">
         <v>0</v>
@@ -1718,7 +1762,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B145">
         <v>0</v>
@@ -1726,7 +1770,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B146">
         <v>0</v>
@@ -1734,7 +1778,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B147">
         <v>0</v>
@@ -1742,7 +1786,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B148">
         <v>0</v>
@@ -1750,7 +1794,7 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B149">
         <v>0</v>
@@ -1758,7 +1802,7 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B150">
         <v>0</v>
@@ -1766,7 +1810,7 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B151">
         <v>0</v>
@@ -1774,7 +1818,7 @@
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B152">
         <v>0</v>
@@ -1782,7 +1826,7 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B153">
         <v>0</v>
@@ -1790,7 +1834,7 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B154">
         <v>0</v>
@@ -1798,7 +1842,7 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B155">
         <v>0</v>
@@ -1806,7 +1850,7 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B156">
         <v>0</v>
@@ -1814,7 +1858,7 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B157">
         <v>0</v>
@@ -1822,7 +1866,7 @@
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B158">
         <v>0</v>
@@ -1830,7 +1874,7 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B159">
         <v>0</v>
@@ -1838,7 +1882,7 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B160">
         <v>0</v>
@@ -1846,7 +1890,7 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B161">
         <v>0</v>
@@ -1854,7 +1898,7 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B162">
         <v>0</v>
@@ -1862,7 +1906,7 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B163">
         <v>0</v>
@@ -1870,7 +1914,7 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B164">
         <v>0</v>
@@ -1878,7 +1922,7 @@
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B165">
         <v>0</v>
@@ -1886,7 +1930,7 @@
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B166">
         <v>0</v>
@@ -1894,7 +1938,7 @@
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B167">
         <v>0</v>
@@ -1902,39 +1946,39 @@
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B168">
-        <v>0</v>
+        <v>31</v>
+      </c>
+      <c r="B168" s="2">
+        <v>43679.639328703706</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B169">
-        <v>0</v>
+        <v>32</v>
+      </c>
+      <c r="B169" s="2">
+        <v>43679.638506944444</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B170">
-        <v>0</v>
+        <v>33</v>
+      </c>
+      <c r="B170" s="2">
+        <v>43679.639513888891</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B171">
-        <v>0</v>
+        <v>34</v>
+      </c>
+      <c r="B171" s="2">
+        <v>43679.639166666668</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B172">
         <v>0</v>
@@ -1942,7 +1986,7 @@
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B173">
         <v>0</v>
@@ -1950,15 +1994,15 @@
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B174">
-        <v>0</v>
+        <v>35</v>
+      </c>
+      <c r="B174" s="2">
+        <v>43679.639849537038</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B175">
         <v>0</v>
@@ -1966,23 +2010,23 @@
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B176">
-        <v>0</v>
+        <v>36</v>
+      </c>
+      <c r="B176" s="2">
+        <v>43679.640393518515</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B177">
-        <v>0</v>
+        <v>37</v>
+      </c>
+      <c r="B177" s="2">
+        <v>43679.640543981484</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B178">
         <v>0</v>
@@ -1990,23 +2034,23 @@
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B179">
-        <v>0</v>
+        <v>38</v>
+      </c>
+      <c r="B179" s="2">
+        <v>43679.640208333331</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B180">
-        <v>0</v>
+        <v>39</v>
+      </c>
+      <c r="B180" s="2">
+        <v>43679.640648148146</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B181">
         <v>0</v>
@@ -2014,7 +2058,7 @@
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B182">
         <v>0</v>
@@ -2022,15 +2066,15 @@
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B183">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="B183" s="2">
+        <v>43679.638182870367</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B184">
         <v>0</v>
@@ -2038,7 +2082,7 @@
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B185">
         <v>0</v>
@@ -2046,15 +2090,15 @@
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B186">
-        <v>0</v>
+        <v>41</v>
+      </c>
+      <c r="B186" s="2">
+        <v>43679.640069444446</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B187">
         <v>0</v>
@@ -2062,7 +2106,7 @@
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B188">
         <v>0</v>
@@ -2070,7 +2114,7 @@
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B189">
         <v>0</v>
@@ -2078,15 +2122,15 @@
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B190">
-        <v>0</v>
+        <v>42</v>
+      </c>
+      <c r="B190" s="2">
+        <v>43679.639039351852</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B191">
         <v>0</v>
@@ -2094,7 +2138,7 @@
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B192">
         <v>0</v>
@@ -2102,15 +2146,15 @@
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B193">
-        <v>0</v>
+        <v>43</v>
+      </c>
+      <c r="B193" s="2">
+        <v>43679.638078703705</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B194">
         <v>0</v>
@@ -2118,7 +2162,7 @@
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B195">
         <v>0</v>
@@ -2126,7 +2170,7 @@
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B196">
         <v>0</v>
@@ -2134,7 +2178,7 @@
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B197">
         <v>0</v>
@@ -2142,7 +2186,7 @@
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B198">
         <v>0</v>
@@ -2150,7 +2194,7 @@
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B199">
         <v>0</v>
@@ -2158,7 +2202,7 @@
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B200">
         <v>0</v>
@@ -2166,7 +2210,7 @@
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B201">
         <v>0</v>
@@ -2174,7 +2218,7 @@
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B202">
         <v>0</v>
@@ -2182,23 +2226,23 @@
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B203">
-        <v>0</v>
+        <v>44</v>
+      </c>
+      <c r="B203" s="2">
+        <v>43679.638796296298</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B204">
-        <v>0</v>
+        <v>45</v>
+      </c>
+      <c r="B204" s="2">
+        <v>43679.638668981483</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B205">
         <v>0</v>
@@ -2206,15 +2250,15 @@
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B206">
-        <v>0</v>
+        <v>46</v>
+      </c>
+      <c r="B206" s="2">
+        <v>43679.63789351852</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B207">
         <v>0</v>
@@ -2222,7 +2266,7 @@
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B208">
         <v>0</v>
@@ -2230,7 +2274,7 @@
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B209">
         <v>0</v>
@@ -2238,7 +2282,7 @@
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B210">
         <v>0</v>
@@ -2246,7 +2290,7 @@
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B211">
         <v>0</v>
@@ -2254,7 +2298,7 @@
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B212">
         <v>0</v>
@@ -2262,7 +2306,7 @@
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B213">
         <v>0</v>
@@ -2270,7 +2314,7 @@
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B214">
         <v>0</v>
@@ -2278,7 +2322,7 @@
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B215">
         <v>0</v>
@@ -2286,7 +2330,7 @@
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B216">
         <v>0</v>
@@ -2294,7 +2338,7 @@
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B217">
         <v>0</v>
@@ -2302,7 +2346,7 @@
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B218">
         <v>0</v>
@@ -2310,7 +2354,7 @@
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B219">
         <v>0</v>
@@ -2318,7 +2362,7 @@
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B220">
         <v>0</v>
@@ -2326,7 +2370,7 @@
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B221">
         <v>0</v>
@@ -2334,7 +2378,7 @@
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B222">
         <v>0</v>
@@ -2342,7 +2386,7 @@
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B223">
         <v>0</v>
@@ -2350,7 +2394,7 @@
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B224">
         <v>0</v>
@@ -2358,7 +2402,7 @@
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B225">
         <v>0</v>
@@ -2366,7 +2410,7 @@
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B226">
         <v>0</v>
@@ -2374,7 +2418,7 @@
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B227">
         <v>0</v>
@@ -2382,7 +2426,7 @@
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B228">
         <v>0</v>
@@ -2390,7 +2434,7 @@
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B229">
         <v>0</v>
@@ -2398,7 +2442,7 @@
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B230">
         <v>0</v>
@@ -2406,7 +2450,7 @@
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B231">
         <v>0</v>
@@ -2414,7 +2458,7 @@
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B232">
         <v>0</v>
@@ -2422,7 +2466,7 @@
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B233">
         <v>0</v>
@@ -2430,7 +2474,7 @@
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B234">
         <v>0</v>
@@ -2438,7 +2482,7 @@
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B235">
         <v>0</v>
@@ -2446,7 +2490,7 @@
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B236">
         <v>0</v>
@@ -2454,7 +2498,7 @@
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B237">
         <v>0</v>
@@ -2462,7 +2506,7 @@
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B238">
         <v>0</v>
@@ -2470,7 +2514,7 @@
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B239">
         <v>0</v>
@@ -2478,7 +2522,7 @@
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B240">
         <v>0</v>
@@ -2486,7 +2530,7 @@
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B241">
         <v>0</v>
@@ -2494,7 +2538,7 @@
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B242">
         <v>0</v>
@@ -2502,7 +2546,7 @@
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B243">
         <v>0</v>
@@ -2510,7 +2554,7 @@
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B244">
         <v>0</v>
@@ -2518,7 +2562,7 @@
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B245">
         <v>0</v>
@@ -2526,7 +2570,7 @@
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B246">
         <v>0</v>
@@ -2534,7 +2578,7 @@
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B247">
         <v>0</v>
@@ -2542,7 +2586,7 @@
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B248">
         <v>0</v>
@@ -2550,7 +2594,7 @@
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B249">
         <v>0</v>
@@ -2558,7 +2602,7 @@
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B250">
         <v>0</v>
@@ -2566,7 +2610,7 @@
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B251">
         <v>0</v>
@@ -2574,7 +2618,7 @@
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B252">
         <v>0</v>
@@ -2582,7 +2626,7 @@
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B253">
         <v>0</v>
@@ -2590,7 +2634,7 @@
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B254">
         <v>0</v>
@@ -2598,7 +2642,7 @@
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B255">
         <v>0</v>
@@ -2606,7 +2650,7 @@
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B256">
         <v>0</v>
@@ -2614,7 +2658,7 @@
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B257">
         <v>0</v>
@@ -2622,7 +2666,7 @@
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B258">
         <v>0</v>
@@ -2630,7 +2674,7 @@
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B259">
         <v>0</v>
@@ -2638,7 +2682,7 @@
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B260">
         <v>0</v>
@@ -2646,7 +2690,7 @@
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B261">
         <v>0</v>
@@ -2654,7 +2698,7 @@
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B262">
         <v>0</v>
@@ -2662,7 +2706,7 @@
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B263">
         <v>0</v>
@@ -2670,7 +2714,7 @@
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B264">
         <v>0</v>
@@ -2678,7 +2722,7 @@
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B265">
         <v>0</v>
@@ -2686,15 +2730,15 @@
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B266">
-        <v>0</v>
+        <v>47</v>
+      </c>
+      <c r="B266" s="2">
+        <v>43679.6408912037</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B267">
         <v>0</v>
@@ -2702,7 +2746,7 @@
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B268">
         <v>0</v>
@@ -2710,7 +2754,7 @@
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B269">
         <v>0</v>
@@ -2718,7 +2762,7 @@
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B270">
         <v>0</v>
@@ -2726,7 +2770,7 @@
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B271">
         <v>0</v>
@@ -2734,15 +2778,15 @@
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B272">
-        <v>0</v>
+        <v>48</v>
+      </c>
+      <c r="B272" s="2">
+        <v>43679.642164351855</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A273" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B273">
         <v>0</v>
@@ -2750,31 +2794,31 @@
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A274" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B274">
-        <v>0</v>
+        <v>49</v>
+      </c>
+      <c r="B274" s="2">
+        <v>43679.642442129632</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A275" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B275">
-        <v>0</v>
+        <v>50</v>
+      </c>
+      <c r="B275" s="2">
+        <v>43679.642256944448</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A276" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B276">
-        <v>0</v>
+        <v>51</v>
+      </c>
+      <c r="B276" s="2">
+        <v>43679.641967592594</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B277">
         <v>0</v>
@@ -2782,7 +2826,7 @@
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B278">
         <v>0</v>
@@ -2790,31 +2834,31 @@
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A279" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B279">
-        <v>0</v>
+        <v>52</v>
+      </c>
+      <c r="B279" s="2">
+        <v>43679.643009259256</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A280" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B280">
-        <v>0</v>
+        <v>53</v>
+      </c>
+      <c r="B280" s="2">
+        <v>43679.642847222225</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A281" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B281">
-        <v>0</v>
+        <v>54</v>
+      </c>
+      <c r="B281" s="2">
+        <v>43679.641134259262</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A282" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B282">
         <v>0</v>
@@ -2822,7 +2866,7 @@
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A283" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B283">
         <v>0</v>
@@ -2830,15 +2874,15 @@
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A284" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B284">
-        <v>0</v>
+        <v>55</v>
+      </c>
+      <c r="B284" s="2">
+        <v>43679.642546296294</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A285" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B285">
         <v>0</v>
@@ -2846,7 +2890,7 @@
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B286">
         <v>0</v>
@@ -2854,7 +2898,7 @@
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A287" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B287">
         <v>0</v>
@@ -2862,7 +2906,7 @@
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A288" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B288">
         <v>0</v>
@@ -2870,7 +2914,7 @@
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B289">
         <v>0</v>
@@ -2878,7 +2922,7 @@
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A290" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B290">
         <v>0</v>
@@ -2886,15 +2930,15 @@
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A291" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B291">
-        <v>0</v>
+        <v>56</v>
+      </c>
+      <c r="B291" s="2">
+        <v>43679.641377314816</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B292">
         <v>0</v>
@@ -2902,7 +2946,7 @@
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A293" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B293">
         <v>0</v>
@@ -2910,7 +2954,7 @@
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A294" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B294">
         <v>0</v>
@@ -2918,7 +2962,7 @@
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A295" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B295">
         <v>0</v>
@@ -2926,7 +2970,7 @@
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A296" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B296">
         <v>0</v>
@@ -2934,7 +2978,7 @@
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A297" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B297">
         <v>0</v>
@@ -2942,7 +2986,7 @@
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A298" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B298">
         <v>0</v>
@@ -2950,7 +2994,7 @@
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A299" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B299">
         <v>0</v>
@@ -2958,7 +3002,7 @@
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A300" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B300">
         <v>0</v>
@@ -2966,7 +3010,7 @@
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A301" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B301">
         <v>0</v>
@@ -2974,7 +3018,7 @@
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A302" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B302">
         <v>0</v>
@@ -2982,7 +3026,7 @@
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A303" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B303">
         <v>0</v>
@@ -2990,7 +3034,7 @@
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A304" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B304">
         <v>0</v>
@@ -2998,7 +3042,7 @@
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A305" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B305">
         <v>0</v>
@@ -3006,7 +3050,7 @@
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A306" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B306">
         <v>0</v>
@@ -3014,7 +3058,7 @@
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A307" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B307">
         <v>0</v>
@@ -3022,7 +3066,7 @@
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A308" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B308">
         <v>0</v>
@@ -3030,7 +3074,7 @@
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A309" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B309">
         <v>0</v>
@@ -3038,7 +3082,7 @@
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A310" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B310">
         <v>0</v>
@@ -3046,7 +3090,7 @@
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A311" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B311">
         <v>0</v>
@@ -3054,7 +3098,7 @@
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A312" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B312">
         <v>0</v>
@@ -3062,7 +3106,7 @@
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A313" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B313">
         <v>0</v>
@@ -3070,7 +3114,7 @@
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A314" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B314">
         <v>0</v>
@@ -3078,7 +3122,7 @@
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A315" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B315">
         <v>0</v>
@@ -3086,7 +3130,7 @@
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A316" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B316">
         <v>0</v>
@@ -3094,7 +3138,7 @@
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A317" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B317">
         <v>0</v>
@@ -3102,7 +3146,7 @@
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A318" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B318">
         <v>0</v>
@@ -3110,7 +3154,7 @@
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A319" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B319">
         <v>0</v>
@@ -3118,7 +3162,7 @@
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A320" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B320">
         <v>0</v>
@@ -3126,7 +3170,7 @@
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A321" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B321">
         <v>0</v>
@@ -3134,7 +3178,7 @@
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A322" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B322">
         <v>0</v>
@@ -3142,7 +3186,7 @@
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A323" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B323">
         <v>0</v>
@@ -3150,7 +3194,7 @@
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A324" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B324">
         <v>0</v>
@@ -3158,7 +3202,7 @@
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A325" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B325">
         <v>0</v>
@@ -3166,7 +3210,7 @@
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A326" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B326">
         <v>0</v>
@@ -3174,7 +3218,7 @@
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A327" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B327">
         <v>0</v>
@@ -3182,7 +3226,7 @@
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A328" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B328">
         <v>0</v>
@@ -3190,7 +3234,7 @@
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A329" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B329">
         <v>0</v>
@@ -3198,7 +3242,7 @@
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A330" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B330">
         <v>0</v>
@@ -3206,7 +3250,7 @@
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A331" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B331">
         <v>0</v>
@@ -3214,7 +3258,7 @@
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A332" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B332">
         <v>0</v>
@@ -3222,7 +3266,7 @@
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A333" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B333">
         <v>0</v>
@@ -3230,7 +3274,7 @@
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A334" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B334">
         <v>0</v>
@@ -3238,7 +3282,7 @@
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A335" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B335">
         <v>0</v>
@@ -3246,7 +3290,7 @@
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A336" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B336">
         <v>0</v>
@@ -3254,7 +3298,7 @@
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A337" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B337">
         <v>0</v>
@@ -3262,10 +3306,130 @@
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A338" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B338">
         <v>0</v>
+      </c>
+    </row>
+    <row r="339" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A339" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B339" s="2">
+        <v>43679.607430555552</v>
+      </c>
+    </row>
+    <row r="340" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A340" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B340" s="2">
+        <v>43679.768148148149</v>
+      </c>
+    </row>
+    <row r="341" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A341" t="s">
+        <v>59</v>
+      </c>
+      <c r="B341" s="3">
+        <v>43680.576585648145</v>
+      </c>
+    </row>
+    <row r="342" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A342" t="s">
+        <v>60</v>
+      </c>
+      <c r="B342" s="3">
+        <v>43680.576689814814</v>
+      </c>
+    </row>
+    <row r="343" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A343" t="s">
+        <v>61</v>
+      </c>
+      <c r="B343" s="3">
+        <v>43680.579259259262</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A344" t="s">
+        <v>62</v>
+      </c>
+      <c r="B344" s="3">
+        <v>43680.579363425924</v>
+      </c>
+    </row>
+    <row r="345" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A345" t="s">
+        <v>63</v>
+      </c>
+      <c r="B345" s="3">
+        <v>43680.579479166663</v>
+      </c>
+    </row>
+    <row r="346" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A346" t="s">
+        <v>64</v>
+      </c>
+      <c r="B346" s="3">
+        <v>43680.579583333332</v>
+      </c>
+    </row>
+    <row r="347" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A347" t="s">
+        <v>65</v>
+      </c>
+      <c r="B347" s="3">
+        <v>43680.579699074071</v>
+      </c>
+    </row>
+    <row r="348" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A348" t="s">
+        <v>66</v>
+      </c>
+      <c r="B348" s="3">
+        <v>43680.57980324074</v>
+      </c>
+    </row>
+    <row r="349" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A349" t="s">
+        <v>67</v>
+      </c>
+      <c r="B349" s="3">
+        <v>43679.630567129629</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A350" t="s">
+        <v>68</v>
+      </c>
+      <c r="B350" s="3">
+        <v>43680.582476851851</v>
+      </c>
+    </row>
+    <row r="351" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A351" t="s">
+        <v>69</v>
+      </c>
+      <c r="B351" s="3">
+        <v>43679.633275462962</v>
+      </c>
+    </row>
+    <row r="352" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A352" t="s">
+        <v>70</v>
+      </c>
+      <c r="B352" s="3">
+        <v>43679.63622685185</v>
+      </c>
+    </row>
+    <row r="353" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A353" t="s">
+        <v>71</v>
+      </c>
+      <c r="B353" s="3">
+        <v>43680.592743055553</v>
       </c>
     </row>
   </sheetData>

</xml_diff>